<commit_message>
Changes to produce visualizations for 2023 report
</commit_message>
<xml_diff>
--- a/bawsvis/examples/annual_stats_norm.xlsx
+++ b/bawsvis/examples/annual_stats_norm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Utveckling\BAWS-vis\bawsvis\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kodning\BAWS-vis\bawsvis\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98495123-65F9-4D66-A577-4647C006F026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB882D53-F827-4ACA-AAC6-85CBDE8766DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="3188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>2021</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -457,22 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -506,7 +509,7 @@
         <v>27408</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -523,7 +526,7 @@
         <v>46016</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -540,7 +543,7 @@
         <v>21407</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -557,7 +560,7 @@
         <v>77674</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -574,7 +577,7 @@
         <v>63421</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -591,7 +594,7 @@
         <v>40392</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -608,7 +611,7 @@
         <v>72501</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -625,7 +628,7 @@
         <v>26331</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -642,7 +645,7 @@
         <v>39972</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -659,7 +662,7 @@
         <v>19876</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -676,7 +679,7 @@
         <v>22075</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -693,7 +696,7 @@
         <v>32410</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -710,7 +713,7 @@
         <v>35821</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -727,7 +730,7 @@
         <v>35033</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -744,7 +747,7 @@
         <v>15804</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -761,7 +764,7 @@
         <v>30263</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -778,7 +781,7 @@
         <v>52049</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -795,7 +798,7 @@
         <v>55195</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -812,7 +815,7 @@
         <v>64873</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -827,6 +830,23 @@
       </c>
       <c r="E21">
         <v>40061</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>246344</v>
+      </c>
+      <c r="C23">
+        <v>7.9</v>
+      </c>
+      <c r="D23">
+        <v>4807</v>
+      </c>
+      <c r="E23">
+        <v>38081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>